<commit_message>
resolve normal outs taking extra variables!
</commit_message>
<xml_diff>
--- a/pujols.xlsx
+++ b/pujols.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="26835" windowHeight="12345"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="21630" windowHeight="9180"/>
   </bookViews>
   <sheets>
     <sheet name="pujols" sheetId="1" r:id="rId1"/>
@@ -713,14 +713,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -1025,10 +1018,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T71"/>
+  <dimension ref="A1:T72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="G72" sqref="G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4912,9 +4905,19 @@
         <v>10</v>
       </c>
     </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="G72">
+        <f>SUM(G2:G71)</f>
+        <v>511</v>
+      </c>
+      <c r="O72">
+        <f>SUM(O2:O71)</f>
+        <v>529</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="I1:L1048576">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",I1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
pujols and turner checks good; batting + fielding
</commit_message>
<xml_diff>
--- a/pujols.xlsx
+++ b/pujols.xlsx
@@ -1219,7 +1219,7 @@
   <dimension ref="A1:BR195"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A125" sqref="A125:G194"/>
     </sheetView>
   </sheetViews>
@@ -8361,7 +8361,7 @@
       <c r="J39" s="24"/>
       <c r="K39" s="24"/>
       <c r="L39" s="24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M39" s="24">
         <v>4</v>
@@ -17925,7 +17925,7 @@
         <v>1</v>
       </c>
       <c r="L89" s="24">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M89" s="24">
         <v>4</v>
@@ -17933,7 +17933,7 @@
       <c r="N89" s="24"/>
       <c r="O89" s="24"/>
       <c r="P89" s="24">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q89" s="24"/>
       <c r="R89" s="24"/>

</xml_diff>